<commit_message>
Added 2006-13 crosstab of pain reliever misuse by state
Source: https://datatools.samhsa.gov/nsduh/2013/nsduh-2006-2013-rd08yr/crosstab?row=STUSAB&column=ANLYR&weight=DASWT_3
</commit_message>
<xml_diff>
--- a/raw_data_kff.xlsx
+++ b/raw_data_kff.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://researchtriangleinstitute-my.sharepoint.com/personal/nbuell_rti_org/Documents/Documents 1/GitHub/data-602-final-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9499082B-9D84-46FC-B0D3-F9D8D5B51213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{9499082B-9D84-46FC-B0D3-F9D8D5B51213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{579A44C5-DA5B-4723-B234-D6F32597CF62}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data_kff" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -763,12 +763,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C55" totalsRowShown="0">
-  <autoFilter ref="A3:C55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:C55" totalsRowShown="0">
+  <autoFilter ref="A3:C55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C55">
+    <sortCondition ref="C3:C55"/>
+  </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Location"/>
-    <tableColumn id="2" name="Status of Medicaid Expansion Decision"/>
-    <tableColumn id="3" name="Implemented Expansion On"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Location"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Status of Medicaid Expansion Decision"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Implemented Expansion On"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1070,7 +1073,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1107,40 +1110,40 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41640</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41640</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>42248</v>
+        <v>41640</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -1151,7 +1154,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1162,7 +1165,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -1173,7 +1176,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1184,7 +1187,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1195,7 +1198,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1206,7 +1209,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -1217,29 +1220,29 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>41640</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>41640</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1250,18 +1253,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>43831</v>
+        <v>41640</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1272,18 +1275,18 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>42036</v>
+        <v>41640</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -1294,18 +1297,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>41640</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -1316,29 +1319,29 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="1">
-        <v>42552</v>
+        <v>41640</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1">
-        <v>43475</v>
+        <v>41640</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1349,7 +1352,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -1360,18 +1363,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="1">
-        <v>41730</v>
+        <v>41640</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
@@ -1382,134 +1385,134 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
+        <v>41730</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="1">
-        <v>44470</v>
+        <v>41866</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="1">
-        <v>42370</v>
+        <v>42005</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="1">
-        <v>44105</v>
+        <v>42036</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="1">
-        <v>41640</v>
+        <v>42248</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="1">
-        <v>41866</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="1">
-        <v>41640</v>
+        <v>42552</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="1">
-        <v>41640</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="1">
-        <v>41640</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="1">
-        <v>45261</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="1">
-        <v>41640</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1">
-        <v>41640</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,43 +1528,43 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="1">
-        <v>41640</v>
+        <v>44470</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="1">
-        <v>42005</v>
+        <v>45108</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="1">
-        <v>41640</v>
+        <v>45261</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
         <v>64</v>
@@ -1569,18 +1572,18 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="1">
-        <v>45108</v>
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -1591,7 +1594,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
@@ -1602,57 +1605,57 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="1">
-        <v>43831</v>
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="1">
-        <v>41640</v>
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="1">
-        <v>43466</v>
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="1">
-        <v>41640</v>
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="1">
-        <v>41640</v>
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>